<commit_message>
finalizado dicionario de dados
</commit_message>
<xml_diff>
--- a/Banco_de_Dados/Dicionario de dados Grupo.xlsx
+++ b/Banco_de_Dados/Dicionario de dados Grupo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Documents\PI\Nova pasta\Health-Analytics\Banco_de_Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA1DA13-F168-47C0-A89E-2FF19287426B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50764BD-F5F3-4F65-81CA-71E8A2B394DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14475" yWindow="4740" windowWidth="12285" windowHeight="9360" xr2:uid="{3D2374EA-0C0B-489D-8F31-401B81372769}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{3D2374EA-0C0B-489D-8F31-401B81372769}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="77">
   <si>
     <t>Tabela Usuario</t>
   </si>
@@ -263,6 +263,31 @@
   </si>
   <si>
     <t xml:space="preserve">Referência á tabela totem. </t>
+  </si>
+  <si>
+    <t>Código do totem</t>
+  </si>
+  <si>
+    <t>IdTotem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto increment e Chave Primária
+</t>
+  </si>
+  <si>
+    <t>Identificador da tabela totem, cada totem tem seu próprio id.</t>
+  </si>
+  <si>
+    <t>Chave estrangeira referencia empresa</t>
+  </si>
+  <si>
+    <t>Chave primária numérico inteiro</t>
+  </si>
+  <si>
+    <t>Preenchimento obrigatório</t>
+  </si>
+  <si>
+    <t>Referêrencia a tabela empresa.</t>
   </si>
 </sst>
 </file>
@@ -696,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B08D83A-6AFB-47A8-9622-B0A36883D957}">
   <dimension ref="A2:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,7 +779,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1171,21 +1196,45 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="4"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="4"/>
+    <row r="35" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E35" s="3">
+        <v>4</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" s="3">
+        <v>4</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="11"/>

</xml_diff>